<commit_message>
Updated to Beta Env
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE961242-8F35-4F33-B601-8DDEE037D2FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60B463-B7E6-4675-9073-477A82B3CE9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
     <sheet name="Reviews_Zoom" sheetId="2" r:id="rId2"/>
     <sheet name="Reviews_AdvancedFilters" sheetId="3" r:id="rId3"/>
-    <sheet name="Sentiment_Filters" sheetId="4" r:id="rId4"/>
-    <sheet name="SortByData" sheetId="5" r:id="rId5"/>
+    <sheet name="Other_Filters" sheetId="6" r:id="rId4"/>
+    <sheet name="Sentiment_Filters" sheetId="4" r:id="rId5"/>
+    <sheet name="SortByData" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -91,9 +92,6 @@
     <t>Content</t>
   </si>
   <si>
-    <t>Keyword</t>
-  </si>
-  <si>
     <t>Tag</t>
   </si>
   <si>
@@ -140,6 +138,15 @@
   </si>
   <si>
     <t>Location Name</t>
+  </si>
+  <si>
+    <t>1,2,3,Recommended,Not Recommended,No Rating</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>and</t>
   </si>
 </sst>
 </file>
@@ -605,23 +612,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -637,15 +643,15 @@
       <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -656,6 +662,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -669,35 +700,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -705,11 +736,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -720,37 +751,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code for content and response filter
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60B463-B7E6-4675-9073-477A82B3CE9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84767E4-C5E4-43E0-A396-6A1B991DDDEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Owner Response</t>
-  </si>
-  <si>
     <t>Rating</t>
   </si>
   <si>
@@ -140,13 +137,25 @@
     <t>Location Name</t>
   </si>
   <si>
-    <t>1,2,3,Recommended,Not Recommended,No Rating</t>
-  </si>
-  <si>
     <t>Keywords</t>
   </si>
   <si>
     <t>and</t>
+  </si>
+  <si>
+    <t>Contents</t>
+  </si>
+  <si>
+    <t>Content, No Content</t>
+  </si>
+  <si>
+    <t>OResponse</t>
+  </si>
+  <si>
+    <t>Response,Draft Response,Assisted Response</t>
+  </si>
+  <si>
+    <t>1,2,3,Recommended,Not Recommended</t>
   </si>
 </sst>
 </file>
@@ -614,16 +623,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,24 +641,30 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -663,26 +678,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -700,35 +725,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -751,37 +776,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1)Updated Test Data File					2)Updated Sentiment Category code to verify					3)Updated Test for sentiment category
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84767E4-C5E4-43E0-A396-6A1B991DDDEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE69E1-6686-4304-AC78-8B7AC447AF08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -156,6 +156,27 @@
   </si>
   <si>
     <t>1,2,3,Recommended,Not Recommended</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Atmosphere</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>MultiSentiment</t>
+  </si>
+  <si>
+    <t>Overall,Atmosphere</t>
   </si>
 </sst>
 </file>
@@ -621,10 +642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,9 +655,10 @@
     <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -652,8 +674,11 @@
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -667,7 +692,10 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -735,25 +765,40 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Review Insights Code
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CE4F7124-51C5-40E1-97BD-1F57330C559E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{635C3553-1D9F-42CF-A56C-C1998657E0CC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" r:id="rId1" sheetId="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Year_YYYY</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -177,13 +174,25 @@
     <t>Overall,Atmosphere,Product,Customer Service,Value</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
     <t>1,2,3,4,5,Recommended,Not Recommended</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Septemper</t>
+  </si>
+  <si>
+    <t>Neural Turing Tech - Primrose, 1131 Steeles Ave. West, M2R 3W8, +14164510870</t>
   </si>
 </sst>
 </file>
@@ -517,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,16 +568,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +591,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,19 +630,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>2020</v>
       </c>
       <c r="D3" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2">
         <v>2020</v>
@@ -652,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -668,42 +677,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -727,18 +736,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -763,50 +772,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -830,42 +839,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -890,34 +899,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated input for DRS
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3FD4FB2E-6CDC-4521-8B35-31FE1E87CD31}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C353B19D-EAFA-4AE8-8207-7CD1C74C1113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reviews_Filter" r:id="rId1" sheetId="1"/>
-    <sheet name="Reviews_Zoom" r:id="rId2" sheetId="2"/>
-    <sheet name="Reviews_AdvancedFilters" r:id="rId3" sheetId="3"/>
-    <sheet name="Other_Filters" r:id="rId4" sheetId="6"/>
-    <sheet name="Sentiment_Filters" r:id="rId5" sheetId="4"/>
-    <sheet name="SortByData" r:id="rId6" sheetId="5"/>
-    <sheet name="Sentiment_Combination" r:id="rId7" sheetId="7"/>
-    <sheet name="Response_Status" r:id="rId8" sheetId="9"/>
-    <sheet name="Global Filters" r:id="rId9" sheetId="8"/>
+    <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
+    <sheet name="Reviews_Zoom" sheetId="2" r:id="rId2"/>
+    <sheet name="Reviews_AdvancedFilters" sheetId="3" r:id="rId3"/>
+    <sheet name="Other_Filters" sheetId="6" r:id="rId4"/>
+    <sheet name="Sentiment_Filters" sheetId="4" r:id="rId5"/>
+    <sheet name="SortByData" sheetId="5" r:id="rId6"/>
+    <sheet name="Sentiment_Combination" sheetId="7" r:id="rId7"/>
+    <sheet name="Response_Status" sheetId="9" r:id="rId8"/>
+    <sheet name="Global Filters" sheetId="8" r:id="rId9"/>
+    <sheet name="Reviews_Insights" sheetId="10" r:id="rId10"/>
+    <sheet name="Displayed_Review_Score" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -219,7 +221,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,21 +256,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -286,10 +287,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -324,7 +325,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -359,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -453,21 +454,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -484,7 +485,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -536,28 +537,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="70.0" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="70" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -601,14 +602,130 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -673,13 +790,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -687,12 +804,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,14 +853,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -751,7 +868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,14 +888,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -786,8 +903,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,14 +956,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -854,7 +971,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -898,14 +1015,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -913,8 +1030,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,15 +1067,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -985,14 +1102,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
-  <dimension ref="A3:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
+  <dimension ref="A3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D5"/>
@@ -1020,6 +1137,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Response Management testng files and test classes
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3E783199-D814-47A9-9F00-85F4DB326F6A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F95D6AE7-DC37-43F3-89A4-5AEDCBE50DD7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="11" firstSheet="8" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" r:id="rId1" sheetId="1"/>
@@ -24,6 +24,7 @@
     <sheet name="Global Filters" r:id="rId9" sheetId="8"/>
     <sheet name="Reviews_Insights" r:id="rId10" sheetId="10"/>
     <sheet name="Displayed_Review_Score" r:id="rId11" sheetId="11"/>
+    <sheet name="Response_Management" r:id="rId12" sheetId="12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -218,6 +219,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
@@ -551,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -827,12 +834,83 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated changes for UI and XLSX comparison
Updated export funtionality
a)Export as CSV
b)Export as XLSX
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F95D6AE7-DC37-43F3-89A4-5AEDCBE50DD7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62E7CF9-DCCE-4D82-8A98-9DB05185B156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="8" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reviews_Filter" r:id="rId1" sheetId="1"/>
-    <sheet name="Reviews_Zoom" r:id="rId2" sheetId="2"/>
-    <sheet name="Reviews_AdvancedFilters" r:id="rId3" sheetId="3"/>
-    <sheet name="Other_Filters" r:id="rId4" sheetId="6"/>
-    <sheet name="Sentiment_Filters" r:id="rId5" sheetId="4"/>
-    <sheet name="SortByData" r:id="rId6" sheetId="5"/>
-    <sheet name="Sentiment_Combination" r:id="rId7" sheetId="7"/>
-    <sheet name="Response_Status" r:id="rId8" sheetId="9"/>
-    <sheet name="Global Filters" r:id="rId9" sheetId="8"/>
-    <sheet name="Reviews_Insights" r:id="rId10" sheetId="10"/>
-    <sheet name="Displayed_Review_Score" r:id="rId11" sheetId="11"/>
-    <sheet name="Response_Management" r:id="rId12" sheetId="12"/>
+    <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
+    <sheet name="Reviews_Zoom" sheetId="2" r:id="rId2"/>
+    <sheet name="Reviews_AdvancedFilters" sheetId="3" r:id="rId3"/>
+    <sheet name="Other_Filters" sheetId="6" r:id="rId4"/>
+    <sheet name="Sentiment_Filters" sheetId="4" r:id="rId5"/>
+    <sheet name="SortByData" sheetId="5" r:id="rId6"/>
+    <sheet name="Sentiment_Combination" sheetId="7" r:id="rId7"/>
+    <sheet name="Response_Status" sheetId="9" r:id="rId8"/>
+    <sheet name="Global Filters" sheetId="8" r:id="rId9"/>
+    <sheet name="Reviews_Insights" sheetId="10" r:id="rId10"/>
+    <sheet name="Displayed_Review_Score" sheetId="11" r:id="rId11"/>
+    <sheet name="Response_Management" sheetId="12" r:id="rId12"/>
+    <sheet name="Quick Response" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -225,14 +226,28 @@
   </si>
   <si>
     <t>February</t>
+  </si>
+  <si>
+    <t>Quick Response Review</t>
+  </si>
+  <si>
+    <t>Nice enough location, plenty of parking, but too far fir me to drive unless i have a good reason.</t>
+  </si>
+  <si>
+    <t>Automation "Quick Responses"</t>
+  </si>
+  <si>
+    <t>AddResponse</t>
+  </si>
+  <si>
+    <t>&lt;b&gt; Thanks for your Review &lt;/b&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +262,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF393939"/>
+      <name val="Open sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,21 +287,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -298,10 +319,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -336,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -371,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -465,21 +486,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -496,7 +517,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -548,31 +569,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="70.0" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="70" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -612,7 +633,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -632,7 +653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -652,7 +673,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -672,7 +693,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -692,7 +713,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -713,25 +734,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="72.85546875" collapsed="true"/>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,7 +772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -772,24 +793,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="72.85546875" collapsed="true"/>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -830,33 +852,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -876,7 +898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -901,33 +923,76 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A56BC0B-983F-498B-931B-808D4E7DFACB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -947,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -972,29 +1037,29 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1014,7 +1079,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1035,25 +1100,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1061,7 +1126,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1070,26 +1135,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1097,7 +1162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1113,7 +1178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1121,7 +1186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1129,7 +1194,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1138,85 +1203,85 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1289,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1232,7 +1297,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1240,7 +1305,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1249,62 +1314,62 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
-  <dimension ref="A3:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
+  <dimension ref="A3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1319,6 +1384,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code for Reviews
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62E7CF9-DCCE-4D82-8A98-9DB05185B156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AF35D1-6D41-42D2-8D35-01FFD3B74312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="Response_Status" sheetId="9" r:id="rId8"/>
     <sheet name="Global Filters" sheetId="8" r:id="rId9"/>
     <sheet name="Reviews_Insights" sheetId="10" r:id="rId10"/>
-    <sheet name="Displayed_Review_Score" sheetId="11" r:id="rId11"/>
-    <sheet name="Response_Management" sheetId="12" r:id="rId12"/>
-    <sheet name="Quick Response" sheetId="13" r:id="rId13"/>
+    <sheet name="Reviews_Feed" sheetId="14" r:id="rId11"/>
+    <sheet name="Displayed_Review_Score" sheetId="11" r:id="rId12"/>
+    <sheet name="Response_Management" sheetId="12" r:id="rId13"/>
+    <sheet name="Quick Response" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -241,6 +242,18 @@
   </si>
   <si>
     <t>&lt;b&gt; Thanks for your Review &lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Thanks for your Review! Automated Response</t>
+  </si>
+  <si>
+    <t>I see that some people have not had a good experience here</t>
   </si>
 </sst>
 </file>
@@ -743,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -799,6 +812,42 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605F602-B94A-4E6E-8CA2-626E068866BA}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -856,7 +905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -927,7 +976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A56BC0B-983F-498B-931B-808D4E7DFACB}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated - adding response to latest reviews
Removed - Unwanted code and classes
</commit_message>
<xml_diff>
--- a/data/Reviews.xlsx
+++ b/data/Reviews.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AF35D1-6D41-42D2-8D35-01FFD3B74312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{FDB09C9D-7F01-470C-8135-26F186F9E9A3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="11" firstSheet="10" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Reviews_Filter" sheetId="1" r:id="rId1"/>
-    <sheet name="Reviews_Zoom" sheetId="2" r:id="rId2"/>
-    <sheet name="Reviews_AdvancedFilters" sheetId="3" r:id="rId3"/>
-    <sheet name="Other_Filters" sheetId="6" r:id="rId4"/>
-    <sheet name="Sentiment_Filters" sheetId="4" r:id="rId5"/>
-    <sheet name="SortByData" sheetId="5" r:id="rId6"/>
-    <sheet name="Sentiment_Combination" sheetId="7" r:id="rId7"/>
-    <sheet name="Response_Status" sheetId="9" r:id="rId8"/>
-    <sheet name="Global Filters" sheetId="8" r:id="rId9"/>
-    <sheet name="Reviews_Insights" sheetId="10" r:id="rId10"/>
-    <sheet name="Reviews_Feed" sheetId="14" r:id="rId11"/>
-    <sheet name="Displayed_Review_Score" sheetId="11" r:id="rId12"/>
-    <sheet name="Response_Management" sheetId="12" r:id="rId13"/>
-    <sheet name="Quick Response" sheetId="13" r:id="rId14"/>
+    <sheet name="Reviews_Filter" r:id="rId1" sheetId="1"/>
+    <sheet name="Reviews_Zoom" r:id="rId2" sheetId="2"/>
+    <sheet name="Reviews_AdvancedFilters" r:id="rId3" sheetId="3"/>
+    <sheet name="Other_Filters" r:id="rId4" sheetId="6"/>
+    <sheet name="Sentiment_Filters" r:id="rId5" sheetId="4"/>
+    <sheet name="SortByData" r:id="rId6" sheetId="5"/>
+    <sheet name="Sentiment_Combination" r:id="rId7" sheetId="7"/>
+    <sheet name="Response_Status" r:id="rId8" sheetId="9"/>
+    <sheet name="Global Filters" r:id="rId9" sheetId="8"/>
+    <sheet name="Reviews_Insights" r:id="rId10" sheetId="10"/>
+    <sheet name="Reviews_Feed" r:id="rId11" sheetId="14"/>
+    <sheet name="Displayed_Review_Score" r:id="rId12" sheetId="11"/>
+    <sheet name="Response_Management" r:id="rId13" sheetId="12"/>
+    <sheet name="Quick Response" r:id="rId14" sheetId="13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -254,12 +254,16 @@
   </si>
   <si>
     <t>I see that some people have not had a good experience here</t>
+  </si>
+  <si>
+    <t>Neural Turing Tech - Greensides, 84 Greensides Ave, M6G 3P7, +1 416-451-0870</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -300,22 +304,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -332,10 +336,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -370,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -405,7 +409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -499,21 +503,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -530,7 +534,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -582,15 +586,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -598,12 +602,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="70" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="70.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -747,14 +751,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C68BF6-FFD7-4A98-9237-0240DAA4816E}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -762,7 +766,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="72.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -806,23 +810,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605F602-B94A-4E6E-8CA2-626E068866BA}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E605F602-B94A-4E6E-8CA2-626E068866BA}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="88.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -842,22 +846,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57FAAA-3BE2-457C-8305-4DBBCB2509DF}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="72.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -897,17 +901,18 @@
         <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D88E4E-AB47-48E0-BB1F-13C07C506551}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -972,13 +977,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A56BC0B-983F-498B-931B-808D4E7DFACB}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A56BC0B-983F-498B-931B-808D4E7DFACB}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -986,9 +991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="80.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="80.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1014,14 +1019,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DB5847-421B-4A8A-A710-C76B70B3EDD4}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F3"/>
@@ -1086,13 +1091,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C124EA-724B-4FDF-8C3B-ACA22E624A0E}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1100,12 +1105,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1149,14 +1154,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A4D02-57DC-4BB7-8D53-929FBBFC505B}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1164,7 +1169,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1184,14 +1189,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8488D843-EE0E-4574-B5A6-E411CE3450F6}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -1199,8 +1204,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1252,14 +1257,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
-  <dimension ref="A1:A8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600401E0-9BAB-41D9-8626-F1E924C78C3E}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1267,7 +1272,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1311,14 +1316,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8772BE-B07C-469C-AABA-000F6294DF3F}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1326,8 +1331,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="49.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1363,13 +1368,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA1A5CF-6452-4CFC-B110-73E642DED634}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1398,14 +1403,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
-  <dimension ref="A3:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B46485-9B97-45E7-AE05-ADBB6B6A9128}">
+  <dimension ref="A3:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D5"/>
@@ -1433,6 +1438,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>